<commit_message>
add next page links
</commit_message>
<xml_diff>
--- a/output/pdex-medicationdispense.xlsx
+++ b/output/pdex-medicationdispense.xlsx
@@ -174,7 +174,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id {[]} {[]}
+    <t xml:space="preserve">id
 </t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>MedicationDispense.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta {[]} {[]}
+    <t xml:space="preserve">Meta
 </t>
   </si>
   <si>
@@ -209,7 +209,7 @@
     <t>MedicationDispense.implicitRules</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -228,7 +228,7 @@
     <t>MedicationDispense.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code {[]} {[]}
+    <t xml:space="preserve">code
 </t>
   </si>
   <si>
@@ -260,7 +260,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative {[]} {[]}
+    <t xml:space="preserve">Narrative
 </t>
   </si>
   <si>
@@ -286,7 +286,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource {[]} {[]}
+    <t xml:space="preserve">Resource
 </t>
   </si>
   <si>
@@ -312,7 +312,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
@@ -347,7 +347,7 @@
     <t>MedicationDispense.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier {[]} {[]}
+    <t xml:space="preserve">Identifier
 </t>
   </si>
   <si>
@@ -375,7 +375,7 @@
     <t>MedicationDispense.partOf</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Procedure]]}
+    <t xml:space="preserve">Reference(Procedure)
 </t>
   </si>
   <si>
@@ -427,8 +427,8 @@
     <t>MedicationDispense.statusReason[x]</t>
   </si>
   <si>
-    <t>CodeableConcept {[]} {[]}
-Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/DetectedIssue]]}</t>
+    <t>CodeableConcept
+Reference(DetectedIssue)</t>
   </si>
   <si>
     <t>Why a dispense was not performed</t>
@@ -455,7 +455,7 @@
     <t>MedicationDispense.category</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
+    <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
@@ -480,8 +480,8 @@
     <t>MedicationDispense.medication[x]</t>
   </si>
   <si>
-    <t>CodeableConcept {[]} {[]}
-Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Medication]]}</t>
+    <t>CodeableConcept
+Reference(Medication)</t>
   </si>
   <si>
     <t>What medication was supplied</t>
@@ -517,7 +517,7 @@
     <t>MedicationDispense.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/Group]]}
+    <t xml:space="preserve">Reference(Patient|Group)
 </t>
   </si>
   <si>
@@ -545,7 +545,7 @@
     <t>MedicationDispense.context</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Encounter], CanonicalType[http://hl7.org/fhir/StructureDefinition/EpisodeOfCare]]}
+    <t xml:space="preserve">Reference(Encounter|EpisodeOfCare)
 </t>
   </si>
   <si>
@@ -564,7 +564,7 @@
     <t>MedicationDispense.supportingInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Resource]]}
+    <t xml:space="preserve">Reference(Resource)
 </t>
   </si>
   <si>
@@ -583,7 +583,7 @@
     <t>MedicationDispense.performer</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement {[]} {[]}
+    <t xml:space="preserve">BackboneElement
 </t>
   </si>
   <si>
@@ -606,7 +606,7 @@
     <t>MedicationDispense.performer.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -672,7 +672,7 @@
     <t>MedicationDispense.performer.actor</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner], CanonicalType[http://hl7.org/fhir/StructureDefinition/PractitionerRole], CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization], CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/Device], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
+    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization|Patient|Device|RelatedPerson)
 </t>
   </si>
   <si>
@@ -691,7 +691,7 @@
     <t>MedicationDispense.location</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Location]]}
+    <t xml:space="preserve">Reference(Location)
 </t>
   </si>
   <si>
@@ -707,7 +707,7 @@
     <t>MedicationDispense.authorizingPrescription</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/MedicationRequest]]}
+    <t xml:space="preserve">Reference(MedicationRequest)
 </t>
   </si>
   <si>
@@ -756,7 +756,7 @@
     <t>MedicationDispense.quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity {[CanonicalType[http://hl7.org/fhir/StructureDefinition/SimpleQuantity]]} {[]}
+    <t xml:space="preserve">Quantity {SimpleQuantity}
 </t>
   </si>
   <si>
@@ -796,7 +796,7 @@
     <t>MedicationDispense.whenPrepared</t>
   </si>
   <si>
-    <t xml:space="preserve">dateTime {[]} {[]}
+    <t xml:space="preserve">dateTime
 </t>
   </si>
   <si>
@@ -851,7 +851,7 @@
     <t>MedicationDispense.receiver</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner]]}
+    <t xml:space="preserve">Reference(Patient|Practitioner)
 </t>
   </si>
   <si>
@@ -870,7 +870,7 @@
     <t>MedicationDispense.note</t>
   </si>
   <si>
-    <t xml:space="preserve">Annotation {[]} {[]}
+    <t xml:space="preserve">Annotation
 </t>
   </si>
   <si>
@@ -892,7 +892,7 @@
     <t>MedicationDispense.dosageInstruction</t>
   </si>
   <si>
-    <t xml:space="preserve">Dosage {[]} {[]}
+    <t xml:space="preserve">Dosage
 </t>
   </si>
   <si>
@@ -936,7 +936,7 @@
     <t>MedicationDispense.substitution.wasSubstituted</t>
   </si>
   <si>
-    <t xml:space="preserve">boolean {[]} {[]}
+    <t xml:space="preserve">boolean
 </t>
   </si>
   <si>
@@ -994,7 +994,7 @@
     <t>MedicationDispense.substitution.responsibleParty</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner], CanonicalType[http://hl7.org/fhir/StructureDefinition/PractitionerRole]]}
+    <t xml:space="preserve">Reference(Practitioner|PractitionerRole)
 </t>
   </si>
   <si>
@@ -1017,7 +1017,7 @@
 Drug Utilization Review (DUR)Alert</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/DetectedIssue]]}
+    <t xml:space="preserve">Reference(DetectedIssue)
 </t>
   </si>
   <si>
@@ -1036,7 +1036,7 @@
     <t>MedicationDispense.eventHistory</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Provenance]]}
+    <t xml:space="preserve">Reference(Provenance)
 </t>
   </si>
   <si>
@@ -1102,67 +1102,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -1198,7 +1198,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO46"/>
+  <dimension ref="A1:AN46"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>

</xml_diff>